<commit_message>
Letzter Tag am Projekt.
</commit_message>
<xml_diff>
--- a/zeitplanung_nando.xlsx
+++ b/zeitplanung_nando.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando.EDP\OneDrive - sluz\Dokumente\Lehre\Adligenswil\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EA1B8C-7127-4978-B80E-23890C34488B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064E099D-7545-4606-A5E6-E70FECE984C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1841,7 +1841,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1850,7 +1850,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2348,8 +2348,8 @@
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="D18" s="41">
         <f>SUM(D19:D33)</f>
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="30"/>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D22" s="80">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
@@ -3948,7 +3948,7 @@
       <c r="U22" s="58"/>
       <c r="V22" s="59"/>
       <c r="W22" s="103">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X22" s="54"/>
       <c r="Y22" s="55"/>
@@ -4152,7 +4152,7 @@
       </c>
       <c r="D25" s="80">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
@@ -4174,9 +4174,11 @@
       <c r="V25" s="59"/>
       <c r="W25" s="108"/>
       <c r="X25" s="103">
+        <v>4</v>
+      </c>
+      <c r="Y25" s="104">
         <v>2</v>
       </c>
-      <c r="Y25" s="104"/>
       <c r="Z25" s="56"/>
       <c r="AA25" s="57"/>
       <c r="AB25" s="98"/>
@@ -4377,7 +4379,7 @@
       </c>
       <c r="D28" s="80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E28" s="49"/>
       <c r="F28" s="50"/>
@@ -4402,7 +4404,9 @@
       <c r="Y28" s="55"/>
       <c r="Z28" s="56"/>
       <c r="AA28" s="57"/>
-      <c r="AB28" s="106"/>
+      <c r="AB28" s="106">
+        <v>4</v>
+      </c>
       <c r="AC28" s="60"/>
       <c r="AD28" s="54"/>
       <c r="AE28" s="88"/>
@@ -4427,7 +4431,9 @@
       <c r="AX28" s="59"/>
       <c r="AY28" s="88"/>
       <c r="AZ28" s="88"/>
-      <c r="BA28" s="55"/>
+      <c r="BA28" s="104">
+        <v>8</v>
+      </c>
       <c r="BB28" s="56"/>
       <c r="BC28" s="57"/>
       <c r="BD28" s="58"/>
@@ -4450,7 +4456,7 @@
       </c>
       <c r="D29" s="80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E29" s="49"/>
       <c r="F29" s="50"/>
@@ -4476,8 +4482,12 @@
       <c r="Z29" s="56"/>
       <c r="AA29" s="57"/>
       <c r="AB29" s="116"/>
-      <c r="AC29" s="107"/>
-      <c r="AD29" s="54"/>
+      <c r="AC29" s="107">
+        <v>8</v>
+      </c>
+      <c r="AD29" s="103">
+        <v>4</v>
+      </c>
       <c r="AE29" s="88"/>
       <c r="AF29" s="89"/>
       <c r="AG29" s="56"/>
@@ -4523,7 +4533,7 @@
       </c>
       <c r="D30" s="80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E30" s="49"/>
       <c r="F30" s="50"/>
@@ -4550,7 +4560,9 @@
       <c r="AA30" s="57"/>
       <c r="AB30" s="101"/>
       <c r="AC30" s="117"/>
-      <c r="AD30" s="103"/>
+      <c r="AD30" s="103">
+        <v>4</v>
+      </c>
       <c r="AE30" s="88"/>
       <c r="AF30" s="89"/>
       <c r="AG30" s="56"/>
@@ -5315,7 +5327,7 @@
       </c>
       <c r="D41" s="41">
         <f>SUM(D42:D44)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E41" s="31"/>
       <c r="F41" s="30"/>
@@ -5386,7 +5398,7 @@
       <c r="C42" s="48"/>
       <c r="D42" s="80">
         <f t="shared" ref="D42:D44" si="3">SUM(G42:BJ42)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="49"/>
       <c r="F42" s="50"/>
@@ -5436,7 +5448,9 @@
       <c r="AX42" s="53"/>
       <c r="AY42" s="88"/>
       <c r="AZ42" s="88"/>
-      <c r="BA42" s="112"/>
+      <c r="BA42" s="112">
+        <v>0.5</v>
+      </c>
       <c r="BB42" s="56"/>
       <c r="BC42" s="57"/>
       <c r="BD42" s="52"/>
@@ -5598,7 +5612,7 @@
       </c>
       <c r="D45" s="36">
         <f>D41+D38+D34+D18+D14+D9</f>
-        <v>36</v>
+        <v>69.5</v>
       </c>
       <c r="E45" s="36"/>
       <c r="F45" s="37"/>
@@ -5668,15 +5682,15 @@
       </c>
       <c r="W45" s="38">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X45" s="38">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Y45" s="38">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z45" s="38">
         <f t="shared" si="4"/>
@@ -5688,15 +5702,15 @@
       </c>
       <c r="AB45" s="38">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AC45" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD45" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE45" s="38">
         <f t="shared" si="4"/>
@@ -5788,7 +5802,7 @@
       </c>
       <c r="BA45" s="38">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="BB45" s="38">
         <f t="shared" si="5"/>
@@ -5930,7 +5944,7 @@
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>
@@ -5979,7 +5993,7 @@
       </c>
       <c r="D8" s="77">
         <f>Zeitplanung!D41</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="78"/>
     </row>

</xml_diff>